<commit_message>
Integrate Agora data for elec/BPaFF
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipE\InputData\elec\BPaFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabian.hein\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C305FAA8-1574-480A-AAA4-AA7C0FFA9348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="23955" windowHeight="10305"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BPaFF-BITPTaP" sheetId="2" r:id="rId2"/>
     <sheet name="BPaFF-BDTPTPF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -152,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,7 +209,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -216,7 +225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -291,6 +300,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -326,6 +352,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -501,12 +544,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -647,15 +692,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
@@ -742,7 +789,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +824,7 @@
       </c>
       <c r="B15">
         <f>B11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -786,7 +833,7 @@
       </c>
       <c r="B16">
         <f>B11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -804,15 +851,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
@@ -827,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +932,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -916,7 +965,7 @@
       </c>
       <c r="B13">
         <f>B2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,7 +1001,7 @@
       </c>
       <c r="B17">
         <f>B9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mark petroleum and heavy or residual fuel oil plants as peakers
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabian.hein\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\elec\BPaFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C305FAA8-1574-480A-AAA4-AA7C0FFA9348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123ACF13-E72E-464A-9A9B-0B95E7139F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BPaFF-BITPTaP" sheetId="2" r:id="rId2"/>
     <sheet name="BPaFF-BDTPTPF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -209,7 +212,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -225,7 +228,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -551,19 +554,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,116 +574,116 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -699,20 +702,20 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -720,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -728,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -736,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -744,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -752,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -760,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -768,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -776,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -784,15 +787,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -800,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -809,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -818,25 +821,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
       <c r="B15">
         <f>B11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16">
-        <f>B11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -861,17 +863,17 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -879,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -887,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -895,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -903,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -911,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -919,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -927,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -935,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -943,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -951,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -959,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -968,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -977,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -986,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -995,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>41</v>
       </c>

</xml_diff>